<commit_message>
scRNAseq mouse data update v0.2 and some analysis workflow added
</commit_message>
<xml_diff>
--- a/src/ScTypeDB_full_Immune_kidney.xlsx
+++ b/src/ScTypeDB_full_Immune_kidney.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\1Research\IgA_Tianyi\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01AD021-A266-4CB2-824A-9C76351659D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520B7A2D-6710-4608-A7D1-50120D336301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -591,9 +591,6 @@
     <t>Regulatory T cell</t>
   </si>
   <si>
-    <t>CCL3L1,CD72,CLEC5A,FOXP3,ITGA4,L1CAM,LIPA,LRP1,LRRC42,MARCO,MMP12,MNDA,MRC1,MS4A6A,PELO,PLEK,PRSS23,PTGIR,ST8SIA4,STAB1</t>
-  </si>
-  <si>
     <t>T follicular helper cell</t>
   </si>
   <si>
@@ -706,6 +703,9 @@
   </si>
   <si>
     <t>CCL18,CD206,CD14,HLA-DR,ARG1,CCL2,CD163,MRC1,RETNLB,IL10,MRC1</t>
+  </si>
+  <si>
+    <t>Il2ra,Cd4,Foxp3,CCL3L1,CD72,CLEC5A,FOXP3,ITGA4,L1CAM,LIPA,LRP1,LRRC42,MARCO,MMP12,MNDA,MRC1,MS4A6A,PELO,PLEK,PRSS23,PTGIR,ST8SIA4,STAB1</t>
   </si>
 </sst>
 </file>
@@ -769,7 +769,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -795,8 +795,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1113,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="76" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="D60" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2084,450 +2083,423 @@
       <c r="B59" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C59" t="s">
         <v>170</v>
       </c>
-      <c r="D59" s="10" t="s">
+      <c r="D59" t="s">
         <v>171</v>
       </c>
       <c r="E59" s="8"/>
-      <c r="F59" s="10"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="C60" t="s">
         <v>172</v>
       </c>
-      <c r="D60" s="10" t="s">
+      <c r="D60" t="s">
         <v>173</v>
       </c>
       <c r="E60" s="8"/>
-      <c r="F60" s="10"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C61" s="10" t="s">
+      <c r="C61" t="s">
         <v>174</v>
       </c>
-      <c r="D61" s="10" t="s">
+      <c r="D61" t="s">
         <v>175</v>
       </c>
       <c r="E61" s="8"/>
-      <c r="F61" s="10"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="C62" t="s">
         <v>176</v>
       </c>
-      <c r="D62" s="10" t="s">
+      <c r="D62" t="s">
         <v>177</v>
       </c>
       <c r="E62" s="8"/>
-      <c r="F62" s="10"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C63" t="s">
         <v>178</v>
       </c>
-      <c r="D63" s="10" t="s">
+      <c r="D63" t="s">
         <v>179</v>
       </c>
       <c r="E63" s="8"/>
-      <c r="F63" s="10"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C64" s="10" t="s">
+      <c r="C64" t="s">
         <v>180</v>
       </c>
-      <c r="D64" s="10" t="s">
+      <c r="D64" t="s">
         <v>181</v>
       </c>
       <c r="E64" s="8"/>
-      <c r="F64" s="10"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C65" s="10" t="s">
+      <c r="C65" t="s">
         <v>182</v>
       </c>
-      <c r="D65" s="10" t="s">
+      <c r="D65" t="s">
         <v>183</v>
       </c>
       <c r="E65" s="8"/>
-      <c r="F65" s="10"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C66" s="10" t="s">
+      <c r="C66" t="s">
         <v>184</v>
       </c>
-      <c r="D66" s="10" t="s">
+      <c r="D66" t="s">
         <v>185</v>
       </c>
       <c r="E66" s="8"/>
-      <c r="F66" s="10"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C67" s="10" t="s">
+      <c r="C67" t="s">
         <v>186</v>
       </c>
-      <c r="D67" s="10" t="s">
-        <v>187</v>
+      <c r="D67" t="s">
+        <v>223</v>
       </c>
       <c r="E67" s="8"/>
-      <c r="F67" s="10"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C68" s="10" t="s">
+      <c r="C68" t="s">
+        <v>187</v>
+      </c>
+      <c r="D68" t="s">
         <v>188</v>
       </c>
-      <c r="D68" s="10" t="s">
-        <v>189</v>
-      </c>
       <c r="E68" s="8"/>
-      <c r="F68" s="10"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C69" s="10" t="s">
+      <c r="C69" t="s">
+        <v>189</v>
+      </c>
+      <c r="D69" t="s">
         <v>190</v>
       </c>
-      <c r="D69" s="10" t="s">
-        <v>191</v>
-      </c>
       <c r="E69" s="8"/>
-      <c r="F69" s="10"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="10" t="s">
+      <c r="C70" t="s">
+        <v>191</v>
+      </c>
+      <c r="D70" t="s">
         <v>192</v>
       </c>
-      <c r="D70" s="10" t="s">
-        <v>193</v>
-      </c>
       <c r="E70" s="8"/>
-      <c r="F70" s="10"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C71" s="10" t="s">
+      <c r="C71" t="s">
+        <v>193</v>
+      </c>
+      <c r="D71" t="s">
         <v>194</v>
       </c>
-      <c r="D71" s="10" t="s">
-        <v>195</v>
-      </c>
       <c r="E71" s="8"/>
-      <c r="F71" s="10"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C72" s="10" t="s">
+      <c r="C72" t="s">
+        <v>195</v>
+      </c>
+      <c r="D72" t="s">
         <v>196</v>
       </c>
-      <c r="D72" s="10" t="s">
-        <v>197</v>
-      </c>
       <c r="E72" s="8"/>
-      <c r="F72" s="10"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C73" s="10" t="s">
+      <c r="C73" t="s">
+        <v>197</v>
+      </c>
+      <c r="D73" t="s">
         <v>198</v>
       </c>
-      <c r="D73" s="10" t="s">
-        <v>199</v>
-      </c>
       <c r="E73" s="8"/>
-      <c r="F73" s="10"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C74" s="10" t="s">
+      <c r="C74" t="s">
+        <v>199</v>
+      </c>
+      <c r="D74" t="s">
         <v>200</v>
       </c>
-      <c r="D74" s="10" t="s">
-        <v>201</v>
-      </c>
       <c r="E74" s="8"/>
-      <c r="F74" s="10"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C75" s="10" t="s">
+      <c r="C75" t="s">
+        <v>201</v>
+      </c>
+      <c r="D75" t="s">
         <v>202</v>
       </c>
-      <c r="D75" s="10" t="s">
-        <v>203</v>
-      </c>
       <c r="E75" s="8"/>
-      <c r="F75" s="10"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C76" s="10" t="s">
+      <c r="C76" t="s">
+        <v>203</v>
+      </c>
+      <c r="D76" t="s">
         <v>204</v>
       </c>
-      <c r="D76" s="10" t="s">
-        <v>205</v>
-      </c>
       <c r="E76" s="8"/>
-      <c r="F76" s="10"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C77" s="10" t="s">
+      <c r="C77" t="s">
+        <v>205</v>
+      </c>
+      <c r="D77" t="s">
         <v>206</v>
       </c>
-      <c r="D77" s="10" t="s">
-        <v>207</v>
-      </c>
       <c r="E77" s="8"/>
-      <c r="F77" s="10"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C78" s="10" t="s">
+      <c r="C78" t="s">
+        <v>207</v>
+      </c>
+      <c r="D78" t="s">
         <v>208</v>
       </c>
-      <c r="D78" s="10" t="s">
-        <v>209</v>
-      </c>
       <c r="E78" s="8"/>
-      <c r="F78" s="10"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C79" s="10" t="s">
+      <c r="C79" t="s">
+        <v>209</v>
+      </c>
+      <c r="D79" t="s">
         <v>210</v>
       </c>
-      <c r="D79" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="E79" s="8"/>
-      <c r="F79" s="10"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C80" s="10" t="s">
+      <c r="C80" t="s">
+        <v>211</v>
+      </c>
+      <c r="D80" t="s">
         <v>212</v>
       </c>
-      <c r="D80" s="10" t="s">
-        <v>213</v>
-      </c>
       <c r="E80" s="8"/>
-      <c r="F80" s="10"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C81" s="10" t="s">
+      <c r="C81" t="s">
+        <v>213</v>
+      </c>
+      <c r="D81" t="s">
         <v>214</v>
       </c>
-      <c r="D81" s="10" t="s">
-        <v>215</v>
-      </c>
       <c r="E81" s="8"/>
-      <c r="F81" s="10"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C82" s="10" t="s">
+      <c r="C82" t="s">
+        <v>215</v>
+      </c>
+      <c r="D82" t="s">
         <v>216</v>
       </c>
-      <c r="D82" s="10" t="s">
-        <v>217</v>
-      </c>
       <c r="E82" s="8"/>
-      <c r="F82" s="10"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C83" s="10" t="s">
+      <c r="C83" t="s">
+        <v>217</v>
+      </c>
+      <c r="D83" t="s">
         <v>218</v>
       </c>
-      <c r="D83" s="10" t="s">
-        <v>219</v>
-      </c>
       <c r="E83" s="8"/>
-      <c r="F83" s="10"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C84" s="10" t="s">
+      <c r="C84" t="s">
+        <v>219</v>
+      </c>
+      <c r="D84" t="s">
         <v>220</v>
       </c>
-      <c r="D84" s="10" t="s">
-        <v>221</v>
-      </c>
       <c r="E84" s="8"/>
-      <c r="F84" s="10"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C85" s="10" t="s">
+      <c r="C85" t="s">
+        <v>221</v>
+      </c>
+      <c r="D85" t="s">
         <v>222</v>
       </c>
-      <c r="D85" s="10" t="s">
-        <v>223</v>
-      </c>
       <c r="E85" s="8"/>
-      <c r="F85" s="10"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>

</xml_diff>